<commit_message>
Connected DB. Added Mailing Controller
</commit_message>
<xml_diff>
--- a/src/main/resources/Book1.xlsx
+++ b/src/main/resources/Book1.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="833" uniqueCount="356">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="833" uniqueCount="358">
   <si>
     <t xml:space="preserve">Шифр</t>
   </si>
@@ -854,10 +854,10 @@
     <t xml:space="preserve"> 211</t>
   </si>
   <si>
-    <t xml:space="preserve"> біологія або математика</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> хімія або фізика</t>
+    <t xml:space="preserve"> біологія або хімія</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> математика або фізика</t>
   </si>
   <si>
     <t xml:space="preserve"> 212</t>
@@ -866,6 +866,37 @@
     <t xml:space="preserve"> Ветеринарна гігієна, санітарія і експертиза</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">математика</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> або фізика</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">22</t>
   </si>
   <si>
@@ -1020,6 +1051,9 @@
   </si>
   <si>
     <t xml:space="preserve"> 263</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> фізика або іноземна мова або хімія або біологія</t>
   </si>
   <si>
     <t xml:space="preserve">27</t>
@@ -1102,7 +1136,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1124,6 +1158,12 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1168,12 +1208,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1196,8 +1240,8 @@
   </sheetPr>
   <dimension ref="A1:G134"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C125" activeCellId="0" sqref="C125"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A110" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G125" activeCellId="0" sqref="G125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1205,7 +1249,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="53.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="21.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="18.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="81.14"/>
@@ -3354,7 +3398,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="105" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B105" s="1" t="s">
         <v>5</v>
       </c>
@@ -3371,21 +3415,21 @@
         <v>276</v>
       </c>
       <c r="G105" s="1" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="1" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="E106" s="1" t="s">
         <v>32</v>
@@ -3394,7 +3438,7 @@
         <v>18</v>
       </c>
       <c r="G106" s="1" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3402,19 +3446,19 @@
         <v>5</v>
       </c>
       <c r="C107" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="D107" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="E107" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F107" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G107" s="1" t="s">
         <v>285</v>
-      </c>
-      <c r="D107" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="E107" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F107" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G107" s="1" t="s">
-        <v>284</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3422,10 +3466,10 @@
         <v>5</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="E108" s="1" t="s">
         <v>32</v>
@@ -3434,7 +3478,7 @@
         <v>18</v>
       </c>
       <c r="G108" s="1" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3442,10 +3486,10 @@
         <v>5</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="E109" s="1" t="s">
         <v>32</v>
@@ -3454,7 +3498,7 @@
         <v>18</v>
       </c>
       <c r="G109" s="1" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3462,10 +3506,10 @@
         <v>5</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="E110" s="1" t="s">
         <v>32</v>
@@ -3474,7 +3518,7 @@
         <v>18</v>
       </c>
       <c r="G110" s="1" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3482,10 +3526,10 @@
         <v>5</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="E111" s="1" t="s">
         <v>32</v>
@@ -3494,7 +3538,7 @@
         <v>18</v>
       </c>
       <c r="G111" s="1" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3502,10 +3546,10 @@
         <v>5</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="E112" s="1" t="s">
         <v>32</v>
@@ -3514,7 +3558,7 @@
         <v>18</v>
       </c>
       <c r="G112" s="1" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3522,10 +3566,10 @@
         <v>5</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="E113" s="1" t="s">
         <v>32</v>
@@ -3534,7 +3578,7 @@
         <v>18</v>
       </c>
       <c r="G113" s="1" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3542,10 +3586,10 @@
         <v>5</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="E114" s="1" t="s">
         <v>32</v>
@@ -3554,21 +3598,21 @@
         <v>18</v>
       </c>
       <c r="G114" s="1" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="1" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="C115" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="D115" s="1" t="s">
         <v>303</v>
-      </c>
-      <c r="D115" s="1" t="s">
-        <v>302</v>
       </c>
       <c r="E115" s="1" t="s">
         <v>13</v>
@@ -3585,10 +3629,10 @@
         <v>5</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="E116" s="1" t="s">
         <v>13</v>
@@ -3602,16 +3646,16 @@
     </row>
     <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="1" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="E117" s="1" t="s">
         <v>13</v>
@@ -3628,10 +3672,10 @@
         <v>5</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="E118" s="1" t="s">
         <v>13</v>
@@ -3645,16 +3689,16 @@
     </row>
     <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="1" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="E119" s="1" t="s">
         <v>32</v>
@@ -3663,7 +3707,7 @@
         <v>18</v>
       </c>
       <c r="G119" s="1" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3671,10 +3715,10 @@
         <v>5</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="E120" s="1" t="s">
         <v>32</v>
@@ -3683,21 +3727,21 @@
         <v>18</v>
       </c>
       <c r="G120" s="1" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="1" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="E121" s="1" t="s">
         <v>32</v>
@@ -3706,7 +3750,7 @@
         <v>18</v>
       </c>
       <c r="G121" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3714,10 +3758,10 @@
         <v>5</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="E122" s="1" t="s">
         <v>32</v>
@@ -3734,10 +3778,10 @@
         <v>5</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="E123" s="1" t="s">
         <v>32</v>
@@ -3754,10 +3798,10 @@
         <v>5</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="E124" s="1" t="s">
         <v>32</v>
@@ -3766,7 +3810,7 @@
         <v>18</v>
       </c>
       <c r="G124" s="1" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3774,10 +3818,10 @@
         <v>5</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="E125" s="1" t="s">
         <v>32</v>
@@ -3786,21 +3830,21 @@
         <v>18</v>
       </c>
       <c r="G125" s="1" t="s">
-        <v>316</v>
+        <v>333</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="1" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="E126" s="1" t="s">
         <v>32</v>
@@ -3809,7 +3853,7 @@
         <v>18</v>
       </c>
       <c r="G126" s="1" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3817,10 +3861,10 @@
         <v>5</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="E127" s="1" t="s">
         <v>32</v>
@@ -3829,18 +3873,18 @@
         <v>18</v>
       </c>
       <c r="G127" s="1" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B128" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="E128" s="1" t="s">
         <v>32</v>
@@ -3848,19 +3892,19 @@
       <c r="F128" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G128" s="1" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G128" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B129" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="E129" s="1" t="s">
         <v>32</v>
@@ -3868,19 +3912,19 @@
       <c r="F129" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G129" s="1" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G129" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B130" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="E130" s="1" t="s">
         <v>32</v>
@@ -3888,22 +3932,22 @@
       <c r="F130" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G130" s="1" t="s">
-        <v>316</v>
+      <c r="G130" s="2" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="1" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="E131" s="1" t="s">
         <v>13</v>
@@ -3917,16 +3961,16 @@
     </row>
     <row r="132" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="1" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="E132" s="1" t="s">
         <v>13</v>
@@ -3943,10 +3987,10 @@
         <v>5</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="E133" s="1" t="s">
         <v>13</v>
@@ -3963,10 +4007,10 @@
         <v>5</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="E134" s="1" t="s">
         <v>13</v>
@@ -3975,13 +4019,13 @@
         <v>26</v>
       </c>
       <c r="G134" s="1" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>